<commit_message>
fixed Equal Representation item
</commit_message>
<xml_diff>
--- a/data/achievements.xlsx
+++ b/data/achievements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/12c59f61e5fb2c22/Desktop/github/root-bingo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1586" documentId="8_{AB9AB7AF-F17D-4125-901F-926F7A193F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{137CB343-034F-43D9-99A5-B429AF127E1B}"/>
+  <xr:revisionPtr revIDLastSave="1589" documentId="8_{AB9AB7AF-F17D-4125-901F-926F7A193F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF115255-2E27-41B0-9159-1BAB5B4BFB04}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3DD2AAD7-0C45-43F7-90C1-2525C62C1F46}"/>
   </bookViews>
@@ -1583,8 +1583,8 @@
   <dimension ref="A1:K161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F152" sqref="F152"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3684,7 +3684,7 @@
         <v>344</v>
       </c>
       <c r="E69" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>

</xml_diff>